<commit_message>
Add System Date format to the import template file and give the ability to user to insert custom date format for the import sheet
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C43442
</commit_message>
<xml_diff>
--- a/TOneV2/Code/TOneV2/TOne.WhS.Sales.Web/WhS_Sales/Templates/Import Rate Plan Template.xlsx
+++ b/TOneV2/Code/TOneV2/TOne.WhS.Sales.Web/WhS_Sales/Templates/Import Rate Plan Template.xlsx
@@ -29,6 +29,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -72,11 +75,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,13 +391,14 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -400,11 +408,12 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Import Rate Plan Template
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C46114
</commit_message>
<xml_diff>
--- a/TOneV2/Code/TOneV2/TOne.WhS.Sales.Web/WhS_Sales/Templates/Import Rate Plan Template.xlsx
+++ b/TOneV2/Code/TOneV2/TOne.WhS.Sales.Web/WhS_Sales/Templates/Import Rate Plan Template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -49,18 +49,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -77,13 +71,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -177,6 +171,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -212,6 +223,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -391,24 +419,24 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added notes for rules
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C48382
</commit_message>
<xml_diff>
--- a/TOneV2/Code/TOneV2/TOne.WhS.Sales.Web/WhS_Sales/Templates/Import Rate Plan Template.xlsx
+++ b/TOneV2/Code/TOneV2/TOne.WhS.Sales.Web/WhS_Sales/Templates/Import Rate Plan Template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -69,14 +69,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -171,23 +174,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -223,23 +209,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -419,7 +388,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,9 +396,10 @@
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.42578125" style="1" customWidth="1"/>
+    <col min="4" max="30" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
implement import routing product in import rate plan
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C49864
</commit_message>
<xml_diff>
--- a/TOneV2/Code/TOneV2/TOne.WhS.Sales.Web/WhS_Sales/Templates/Import Rate Plan Template.xlsx
+++ b/TOneV2/Code/TOneV2/TOne.WhS.Sales.Web/WhS_Sales/Templates/Import Rate Plan Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Zone</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>Effective Date</t>
+  </si>
+  <si>
+    <t>Routing Product</t>
   </si>
 </sst>
 </file>
@@ -385,11 +388,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -399,7 +400,7 @@
     <col min="4" max="30" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -409,6 +410,9 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>